<commit_message>
Reformatted filenames to standardize and simplify, updated with new jurisdictions
</commit_message>
<xml_diff>
--- a/ZoningAtlas/raw_data/zoning_needs_to_join/Windsor_Weston_features.xlsx
+++ b/ZoningAtlas/raw_data/zoning_needs_to_join/Windsor_Weston_features.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ybird/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ybird/ZoningAtlas/VT_Zoning_Atlas/ZoningAtlas/raw_data/zoning_needs_to_join/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0513FCF-80B2-1D48-A414-E32779D89DB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC1C8151-1024-A04F-9A4C-E2A10A4F88A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1300" yWindow="840" windowWidth="29400" windowHeight="18400" activeTab="1" xr2:uid="{FC763E2B-1BB8-D248-8DD1-F66FE797A262}"/>
+    <workbookView xWindow="1300" yWindow="840" windowWidth="29400" windowHeight="18400" xr2:uid="{FC763E2B-1BB8-D248-8DD1-F66FE797A262}"/>
   </bookViews>
   <sheets>
     <sheet name="Districts" sheetId="1" r:id="rId1"/>
@@ -470,8 +470,8 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1284,13 +1284,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB4BA41B-4280-B747-9B6E-C79D73F6A3E5}">
-  <dimension ref="A1:T144"/>
+  <dimension ref="A1:O144"/>
   <sheetViews>
-    <sheetView zoomScale="125" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="L2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="R18" sqref="R18"/>
+      <selection pane="bottomRight" activeCell="P1" sqref="P1:T1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1310,11 +1310,9 @@
     <col min="13" max="13" width="14.83203125" customWidth="1"/>
     <col min="14" max="14" width="14.83203125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="14.83203125" customWidth="1"/>
-    <col min="16" max="19" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="26.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>2</v>
       </c>
@@ -1360,13 +1358,8 @@
       <c r="O1" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="P1" s="3"/>
-      <c r="Q1" s="3"/>
-      <c r="R1" s="3"/>
-      <c r="S1" s="3"/>
-      <c r="T1" s="3"/>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1399,7 +1392,7 @@
       </c>
       <c r="O2" s="1"/>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -1432,7 +1425,7 @@
       </c>
       <c r="O3" s="1"/>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -1465,7 +1458,7 @@
       </c>
       <c r="O4" s="1"/>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -1498,7 +1491,7 @@
       </c>
       <c r="O5" s="1"/>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -1531,7 +1524,7 @@
       </c>
       <c r="O6" s="1"/>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -1564,7 +1557,7 @@
       </c>
       <c r="O7" s="1"/>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -1597,7 +1590,7 @@
       </c>
       <c r="O8" s="1"/>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -1630,7 +1623,7 @@
       </c>
       <c r="O9" s="1"/>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -1663,7 +1656,7 @@
       </c>
       <c r="O10" s="1"/>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>17</v>
       </c>
@@ -1696,7 +1689,7 @@
       </c>
       <c r="O11" s="1"/>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>18</v>
       </c>
@@ -1729,7 +1722,7 @@
       </c>
       <c r="O12" s="1"/>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>19</v>
       </c>
@@ -1762,7 +1755,7 @@
       </c>
       <c r="O13" s="1"/>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>20</v>
       </c>
@@ -1795,7 +1788,7 @@
       </c>
       <c r="O14" s="1"/>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>21</v>
       </c>
@@ -1828,7 +1821,7 @@
       </c>
       <c r="O15" s="1"/>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>22</v>
       </c>
@@ -1861,7 +1854,7 @@
       </c>
       <c r="O16" s="1"/>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>23</v>
       </c>
@@ -1894,7 +1887,7 @@
       </c>
       <c r="O17" s="1"/>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>24</v>
       </c>
@@ -1927,7 +1920,7 @@
       </c>
       <c r="O18" s="1"/>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>68</v>
       </c>
@@ -1939,7 +1932,7 @@
       <c r="M19" s="1"/>
       <c r="O19" s="1"/>
     </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>35</v>
       </c>
@@ -1957,13 +1950,8 @@
       <c r="M20" s="1"/>
       <c r="N20" s="1"/>
       <c r="O20" s="1"/>
-      <c r="P20" s="1"/>
-      <c r="Q20" s="1"/>
-      <c r="R20" s="1"/>
-      <c r="S20" s="1"/>
-      <c r="T20" s="1"/>
-    </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.2">
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>36</v>
       </c>
@@ -2010,7 +1998,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>25</v>
       </c>
@@ -2057,7 +2045,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>26</v>
       </c>
@@ -2104,7 +2092,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>27</v>
       </c>
@@ -2151,7 +2139,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>28</v>
       </c>
@@ -2198,7 +2186,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>29</v>
       </c>
@@ -2224,7 +2212,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>30</v>
       </c>
@@ -2250,7 +2238,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>31</v>
       </c>
@@ -2297,7 +2285,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>32</v>
       </c>
@@ -2344,7 +2332,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>33</v>
       </c>
@@ -2391,7 +2379,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>34</v>
       </c>
@@ -2417,7 +2405,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>43</v>
       </c>
@@ -2443,7 +2431,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="33" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
         <v>37</v>
       </c>
@@ -2461,13 +2449,8 @@
       <c r="M33" s="1"/>
       <c r="N33" s="1"/>
       <c r="O33" s="1"/>
-      <c r="P33" s="1"/>
-      <c r="Q33" s="1"/>
-      <c r="R33" s="1"/>
-      <c r="S33" s="1"/>
-      <c r="T33" s="1"/>
-    </row>
-    <row r="34" spans="1:20" x14ac:dyDescent="0.2">
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>41</v>
       </c>
@@ -2497,7 +2480,7 @@
       </c>
       <c r="O34" s="1"/>
     </row>
-    <row r="35" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>42</v>
       </c>
@@ -2527,7 +2510,7 @@
       </c>
       <c r="O35" s="1"/>
     </row>
-    <row r="36" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>36</v>
       </c>
@@ -2571,7 +2554,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="37" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>91</v>
       </c>
@@ -2615,7 +2598,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="38" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>25</v>
       </c>
@@ -2659,7 +2642,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="39" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>26</v>
       </c>
@@ -2703,7 +2686,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="40" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>27</v>
       </c>
@@ -2747,7 +2730,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="41" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>28</v>
       </c>
@@ -2791,7 +2774,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="42" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>29</v>
       </c>
@@ -2817,7 +2800,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="43" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>30</v>
       </c>
@@ -2843,7 +2826,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="44" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>44</v>
       </c>
@@ -2887,7 +2870,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="45" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>45</v>
       </c>
@@ -2931,7 +2914,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="46" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>32</v>
       </c>
@@ -2975,7 +2958,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="47" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>33</v>
       </c>
@@ -3019,7 +3002,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="48" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>34</v>
       </c>
@@ -3045,7 +3028,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="49" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>43</v>
       </c>
@@ -3071,7 +3054,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="50" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="s">
         <v>38</v>
       </c>
@@ -3089,13 +3072,8 @@
       <c r="M50" s="1"/>
       <c r="N50" s="1"/>
       <c r="O50" s="1"/>
-      <c r="P50" s="1"/>
-      <c r="Q50" s="1"/>
-      <c r="R50" s="1"/>
-      <c r="S50" s="1"/>
-      <c r="T50" s="1"/>
-    </row>
-    <row r="51" spans="1:20" x14ac:dyDescent="0.2">
+    </row>
+    <row r="51" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>41</v>
       </c>
@@ -3122,7 +3100,7 @@
       </c>
       <c r="O51" s="1"/>
     </row>
-    <row r="52" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>42</v>
       </c>
@@ -3149,7 +3127,7 @@
       </c>
       <c r="O52" s="1"/>
     </row>
-    <row r="53" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>36</v>
       </c>
@@ -3190,7 +3168,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="54" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>91</v>
       </c>
@@ -3231,7 +3209,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="55" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>25</v>
       </c>
@@ -3272,7 +3250,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="56" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>26</v>
       </c>
@@ -3313,7 +3291,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="57" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>27</v>
       </c>
@@ -3354,7 +3332,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="58" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>28</v>
       </c>
@@ -3395,7 +3373,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="59" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>29</v>
       </c>
@@ -3421,7 +3399,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="60" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>30</v>
       </c>
@@ -3447,7 +3425,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="61" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>44</v>
       </c>
@@ -3488,7 +3466,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="62" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>45</v>
       </c>
@@ -3529,7 +3507,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="63" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>46</v>
       </c>
@@ -3556,7 +3534,7 @@
       </c>
       <c r="O63" s="1"/>
     </row>
-    <row r="64" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>47</v>
       </c>
@@ -3583,7 +3561,7 @@
       </c>
       <c r="O64" s="1"/>
     </row>
-    <row r="65" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>32</v>
       </c>
@@ -3624,7 +3602,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="66" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>33</v>
       </c>
@@ -3665,7 +3643,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="67" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>34</v>
       </c>
@@ -3691,7 +3669,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="68" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>43</v>
       </c>
@@ -3717,7 +3695,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="69" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>48</v>
       </c>
@@ -3743,7 +3721,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="70" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A70" s="2" t="s">
         <v>39</v>
       </c>
@@ -3775,13 +3753,8 @@
       <c r="O70" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="P70" s="1"/>
-      <c r="Q70" s="1"/>
-      <c r="R70" s="1"/>
-      <c r="S70" s="1"/>
-      <c r="T70" s="1"/>
-    </row>
-    <row r="71" spans="1:20" x14ac:dyDescent="0.2">
+    </row>
+    <row r="71" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>41</v>
       </c>
@@ -3808,7 +3781,7 @@
       </c>
       <c r="O71" s="1"/>
     </row>
-    <row r="72" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>42</v>
       </c>
@@ -3835,7 +3808,7 @@
       </c>
       <c r="O72" s="1"/>
     </row>
-    <row r="73" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>36</v>
       </c>
@@ -3876,7 +3849,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="74" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>91</v>
       </c>
@@ -3917,7 +3890,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="75" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>25</v>
       </c>
@@ -3958,7 +3931,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="76" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>26</v>
       </c>
@@ -3999,7 +3972,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="77" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>27</v>
       </c>
@@ -4040,7 +4013,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="78" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>28</v>
       </c>
@@ -4081,7 +4054,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="79" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>29</v>
       </c>
@@ -4107,7 +4080,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="80" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>30</v>
       </c>
@@ -4133,7 +4106,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="81" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>44</v>
       </c>
@@ -4174,7 +4147,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="82" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>45</v>
       </c>
@@ -4215,7 +4188,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="83" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>46</v>
       </c>
@@ -4242,7 +4215,7 @@
       </c>
       <c r="O83" s="1"/>
     </row>
-    <row r="84" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>47</v>
       </c>
@@ -4269,7 +4242,7 @@
       </c>
       <c r="O84" s="1"/>
     </row>
-    <row r="85" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>32</v>
       </c>
@@ -4310,7 +4283,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="86" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>33</v>
       </c>
@@ -4351,7 +4324,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="87" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>34</v>
       </c>
@@ -4377,7 +4350,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="88" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>43</v>
       </c>
@@ -4403,7 +4376,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="89" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>48</v>
       </c>
@@ -4429,7 +4402,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="90" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>49</v>
       </c>
@@ -4455,7 +4428,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="91" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A91" s="2" t="s">
         <v>40</v>
       </c>
@@ -4487,13 +4460,8 @@
       <c r="O91" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="P91" s="1"/>
-      <c r="Q91" s="1"/>
-      <c r="R91" s="1"/>
-      <c r="S91" s="1"/>
-      <c r="T91" s="1"/>
-    </row>
-    <row r="92" spans="1:20" x14ac:dyDescent="0.2">
+    </row>
+    <row r="92" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>41</v>
       </c>
@@ -4520,7 +4488,7 @@
       </c>
       <c r="O92" s="1"/>
     </row>
-    <row r="93" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>42</v>
       </c>
@@ -4547,7 +4515,7 @@
       </c>
       <c r="O93" s="1"/>
     </row>
-    <row r="94" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>36</v>
       </c>
@@ -4588,7 +4556,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="95" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>91</v>
       </c>
@@ -4629,7 +4597,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="96" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>25</v>
       </c>
@@ -4670,7 +4638,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="97" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>26</v>
       </c>
@@ -4711,7 +4679,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="98" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>27</v>
       </c>
@@ -4752,7 +4720,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="99" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>28</v>
       </c>
@@ -4793,7 +4761,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="100" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>29</v>
       </c>
@@ -4819,7 +4787,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="101" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>30</v>
       </c>
@@ -4845,7 +4813,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="102" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>44</v>
       </c>
@@ -4886,7 +4854,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="103" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>45</v>
       </c>
@@ -4927,7 +4895,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="104" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>46</v>
       </c>
@@ -4954,7 +4922,7 @@
       </c>
       <c r="O104" s="1"/>
     </row>
-    <row r="105" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>47</v>
       </c>
@@ -4981,7 +4949,7 @@
       </c>
       <c r="O105" s="1"/>
     </row>
-    <row r="106" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>32</v>
       </c>
@@ -5022,7 +4990,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="107" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>33</v>
       </c>
@@ -5063,7 +5031,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="108" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>34</v>
       </c>
@@ -5089,7 +5057,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="109" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>43</v>
       </c>
@@ -5115,7 +5083,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="110" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>48</v>
       </c>
@@ -5141,7 +5109,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="111" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>49</v>
       </c>
@@ -5167,7 +5135,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="112" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A112" s="2" t="s">
         <v>50</v>
       </c>
@@ -5199,37 +5167,27 @@
       <c r="O112" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="P112" s="1"/>
-      <c r="Q112" s="1"/>
-      <c r="R112" s="1"/>
-      <c r="S112" s="1"/>
-      <c r="T112" s="1"/>
-    </row>
-    <row r="113" spans="1:20" x14ac:dyDescent="0.2">
+    </row>
+    <row r="113" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>51</v>
       </c>
-      <c r="B113" s="5"/>
-      <c r="C113" s="5"/>
-      <c r="D113" s="5"/>
-      <c r="E113" s="5"/>
-      <c r="F113" s="5"/>
-      <c r="G113" s="5"/>
-      <c r="H113" s="5"/>
-      <c r="I113" s="5"/>
-      <c r="J113" s="5"/>
-      <c r="K113" s="5"/>
-      <c r="L113" s="5"/>
-      <c r="M113" s="5"/>
-      <c r="N113" s="5"/>
-      <c r="O113" s="5"/>
-      <c r="P113" s="5"/>
-      <c r="Q113" s="5"/>
-      <c r="R113" s="5"/>
-      <c r="S113" s="5"/>
-      <c r="T113" s="5"/>
-    </row>
-    <row r="114" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="B113" s="6"/>
+      <c r="C113" s="6"/>
+      <c r="D113" s="6"/>
+      <c r="E113" s="6"/>
+      <c r="F113" s="6"/>
+      <c r="G113" s="6"/>
+      <c r="H113" s="6"/>
+      <c r="I113" s="6"/>
+      <c r="J113" s="6"/>
+      <c r="K113" s="6"/>
+      <c r="L113" s="6"/>
+      <c r="M113" s="6"/>
+      <c r="N113" s="6"/>
+      <c r="O113" s="6"/>
+    </row>
+    <row r="114" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>42</v>
       </c>
@@ -5241,7 +5199,7 @@
       <c r="M114" s="1"/>
       <c r="O114" s="1"/>
     </row>
-    <row r="115" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>36</v>
       </c>
@@ -5267,7 +5225,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="116" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>91</v>
       </c>
@@ -5293,7 +5251,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="117" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>44</v>
       </c>
@@ -5319,7 +5277,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="118" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>45</v>
       </c>
@@ -5345,7 +5303,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="119" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>43</v>
       </c>
@@ -5371,7 +5329,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="120" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>48</v>
       </c>
@@ -5397,7 +5355,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="121" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>49</v>
       </c>
@@ -5423,7 +5381,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="122" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A122" s="2" t="s">
         <v>52</v>
       </c>
@@ -5455,13 +5413,8 @@
       <c r="O122" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="P122" s="1"/>
-      <c r="Q122" s="1"/>
-      <c r="R122" s="1"/>
-      <c r="S122" s="1"/>
-      <c r="T122" s="1"/>
-    </row>
-    <row r="123" spans="1:20" x14ac:dyDescent="0.2">
+    </row>
+    <row r="123" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>53</v>
       </c>
@@ -5494,7 +5447,7 @@
       </c>
       <c r="O123" s="1"/>
     </row>
-    <row r="124" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>54</v>
       </c>
@@ -5527,7 +5480,7 @@
       </c>
       <c r="O124" s="1"/>
     </row>
-    <row r="125" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>55</v>
       </c>
@@ -5560,7 +5513,7 @@
       </c>
       <c r="O125" s="1"/>
     </row>
-    <row r="126" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>42</v>
       </c>
@@ -5593,7 +5546,7 @@
       </c>
       <c r="O126" s="1"/>
     </row>
-    <row r="127" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>36</v>
       </c>
@@ -5640,7 +5593,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="128" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>31</v>
       </c>
@@ -5687,7 +5640,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="129" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>56</v>
       </c>
@@ -5720,7 +5673,7 @@
       </c>
       <c r="O129" s="1"/>
     </row>
-    <row r="130" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>57</v>
       </c>
@@ -5767,7 +5720,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="131" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>58</v>
       </c>
@@ -5793,7 +5746,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="132" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>48</v>
       </c>
@@ -5840,7 +5793,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="133" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A133" s="2" t="s">
         <v>59</v>
       </c>
@@ -5872,13 +5825,8 @@
       <c r="O133" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="P133" s="1"/>
-      <c r="Q133" s="1"/>
-      <c r="R133" s="1"/>
-      <c r="S133" s="1"/>
-      <c r="T133" s="1"/>
-    </row>
-    <row r="134" spans="1:20" x14ac:dyDescent="0.2">
+    </row>
+    <row r="134" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
         <v>60</v>
       </c>
@@ -5905,7 +5853,7 @@
       </c>
       <c r="O134" s="1"/>
     </row>
-    <row r="135" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
         <v>36</v>
       </c>
@@ -5931,7 +5879,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="136" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
         <v>91</v>
       </c>
@@ -5972,7 +5920,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="137" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
         <v>61</v>
       </c>
@@ -5984,7 +5932,7 @@
       <c r="M137" s="1"/>
       <c r="O137" s="1"/>
     </row>
-    <row r="138" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A138" s="2" t="s">
         <v>62</v>
       </c>
@@ -6016,13 +5964,8 @@
       <c r="O138" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="P138" s="1"/>
-      <c r="Q138" s="1"/>
-      <c r="R138" s="1"/>
-      <c r="S138" s="1"/>
-      <c r="T138" s="1"/>
-    </row>
-    <row r="139" spans="1:20" x14ac:dyDescent="0.2">
+    </row>
+    <row r="139" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
         <v>63</v>
       </c>
@@ -6034,7 +5977,7 @@
       <c r="M139" s="1"/>
       <c r="O139" s="1"/>
     </row>
-    <row r="140" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
         <v>64</v>
       </c>
@@ -6046,7 +5989,7 @@
       <c r="M140" s="1"/>
       <c r="O140" s="1"/>
     </row>
-    <row r="141" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
         <v>65</v>
       </c>
@@ -6058,7 +6001,7 @@
       <c r="M141" s="1"/>
       <c r="O141" s="1"/>
     </row>
-    <row r="142" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
         <v>66</v>
       </c>
@@ -6070,7 +6013,7 @@
       <c r="M142" s="1"/>
       <c r="O142" s="1"/>
     </row>
-    <row r="143" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A143" s="2" t="s">
         <v>67</v>
       </c>
@@ -6102,13 +6045,8 @@
       <c r="O143" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="P143" s="1"/>
-      <c r="Q143" s="1"/>
-      <c r="R143" s="1"/>
-      <c r="S143" s="1"/>
-      <c r="T143" s="1"/>
-    </row>
-    <row r="144" spans="1:20" x14ac:dyDescent="0.2">
+    </row>
+    <row r="144" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
         <v>95</v>
       </c>
@@ -6136,361 +6074,361 @@
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B113:T113"/>
+    <mergeCell ref="B113:O113"/>
   </mergeCells>
-  <conditionalFormatting sqref="B34:B35 D34:D35 J34:J37 F34:F49 H34:H49 L34:L49 N34:N49 K36:K37 B36:E49 G36:G49 I36:I49 M36:M49 O36:O49 J44:K49 P34:T49">
+  <conditionalFormatting sqref="B34:B35 D34:D35 J34:J37 F34:F49 H34:H49 L34:L49 N34:N49 K36:K37 B36:E49 G36:G49 I36:I49 M36:M49 O36:O49 J44:K49">
     <cfRule type="expression" dxfId="70" priority="278">
       <formula>OR(B$12="", B$12="Prohibited")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B51:B52 D51:D52 J51:J54 L51:L69 N51:N69 K53:K54 B53:E62 M53:M62 O53:O62 K61:K62 J61:J69 B63:B64 D63:D64 B65:E69 G65:G69 I65:I69 K65:K69 M65:M69 O65:O69 F67:F69 H67:H69 P51:T69">
+  <conditionalFormatting sqref="B51:B52 D51:D52 J51:J54 L51:L69 N51:N69 K53:K54 B53:E62 M53:M62 O53:O62 K61:K62 J61:J69 B63:B64 D63:D64 B65:E69 G65:G69 I65:I69 K65:K69 M65:M69 O65:O69 F67:F69 H67:H69">
     <cfRule type="expression" dxfId="69" priority="277" stopIfTrue="1">
       <formula>OR(B$13="", B$13="Prohibited")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B21:T32">
-    <cfRule type="expression" dxfId="68" priority="279" stopIfTrue="1">
+  <conditionalFormatting sqref="B114:B121 D114:D121 F114:F121 H114:H121 J114:J121 L114:L121 N114:N121">
+    <cfRule type="expression" dxfId="68" priority="274" stopIfTrue="1">
+      <formula>OR(B$17="", B$17="Prohibited")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B123:B132 D123:D132 F123:F132 H123:H132 J123:J132 L123:L132 N123:N132">
+    <cfRule type="expression" dxfId="67" priority="273">
+      <formula>OR(B$16="", B$16="Prohibited")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B134:B137 D134:D137 F134:F137 H134:H137 J134:J137 L134:L137 N134:N137">
+    <cfRule type="expression" dxfId="66" priority="272" stopIfTrue="1">
+      <formula>OR(B$18="Prohibited", B$18="")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B21:O32">
+    <cfRule type="expression" dxfId="65" priority="279" stopIfTrue="1">
       <formula>OR(B$11="", B$11="Prohibited")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C73:C82 C85:C89">
-    <cfRule type="expression" dxfId="67" priority="271" stopIfTrue="1">
+    <cfRule type="expression" dxfId="64" priority="271" stopIfTrue="1">
       <formula>OR(C$13="", C$13="Prohibited")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C94:C103 C106:C110">
-    <cfRule type="expression" dxfId="66" priority="269" stopIfTrue="1">
+    <cfRule type="expression" dxfId="63" priority="269" stopIfTrue="1">
       <formula>OR(C$13="", C$13="Prohibited")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C111">
-    <cfRule type="expression" dxfId="65" priority="270">
+    <cfRule type="expression" dxfId="62" priority="270">
       <formula>OR(C$14="", C$14="Prohibited")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C115:C120">
-    <cfRule type="expression" dxfId="64" priority="262" stopIfTrue="1">
+    <cfRule type="expression" dxfId="61" priority="262" stopIfTrue="1">
       <formula>OR(C$13="", C$13="Prohibited")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C121">
-    <cfRule type="expression" dxfId="63" priority="263">
+    <cfRule type="expression" dxfId="60" priority="263">
       <formula>OR(C$14="", C$14="Prohibited")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C127:C128">
-    <cfRule type="expression" dxfId="62" priority="260" stopIfTrue="1">
+    <cfRule type="expression" dxfId="59" priority="260" stopIfTrue="1">
       <formula>OR(C$13="", C$13="Prohibited")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C130:C132">
-    <cfRule type="expression" dxfId="61" priority="257" stopIfTrue="1">
+    <cfRule type="expression" dxfId="58" priority="257" stopIfTrue="1">
       <formula>OR(C$13="", C$13="Prohibited")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C135:C136">
-    <cfRule type="expression" dxfId="60" priority="255" stopIfTrue="1">
+    <cfRule type="expression" dxfId="57" priority="255" stopIfTrue="1">
       <formula>OR(C$13="", C$13="Prohibited")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E73:E82 E85:E89">
-    <cfRule type="expression" dxfId="59" priority="101" stopIfTrue="1">
+    <cfRule type="expression" dxfId="56" priority="101" stopIfTrue="1">
       <formula>OR(E$13="", E$13="Prohibited")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E94:E103 E106:E110">
-    <cfRule type="expression" dxfId="58" priority="99" stopIfTrue="1">
+    <cfRule type="expression" dxfId="55" priority="99" stopIfTrue="1">
       <formula>OR(E$13="", E$13="Prohibited")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E115:E120">
-    <cfRule type="expression" dxfId="57" priority="97" stopIfTrue="1">
+    <cfRule type="expression" dxfId="54" priority="97" stopIfTrue="1">
       <formula>OR(E$13="", E$13="Prohibited")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E121">
-    <cfRule type="expression" dxfId="56" priority="98">
+    <cfRule type="expression" dxfId="53" priority="98">
       <formula>OR(E$14="", E$14="Prohibited")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E127:E128">
-    <cfRule type="expression" dxfId="55" priority="53" stopIfTrue="1">
+    <cfRule type="expression" dxfId="52" priority="53" stopIfTrue="1">
       <formula>OR(E$13="", E$13="Prohibited")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E130:E132">
-    <cfRule type="expression" dxfId="54" priority="52" stopIfTrue="1">
+    <cfRule type="expression" dxfId="51" priority="52" stopIfTrue="1">
       <formula>OR(E$13="", E$13="Prohibited")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E135:E136">
-    <cfRule type="expression" dxfId="53" priority="94" stopIfTrue="1">
+    <cfRule type="expression" dxfId="50" priority="94" stopIfTrue="1">
       <formula>OR(E$13="", E$13="Prohibited")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E111:I111">
-    <cfRule type="expression" dxfId="52" priority="11">
+    <cfRule type="expression" dxfId="49" priority="11">
       <formula>OR(E$14="", E$14="Prohibited")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F51:F66 G53:G62">
-    <cfRule type="expression" dxfId="51" priority="40">
+    <cfRule type="expression" dxfId="48" priority="40">
       <formula>OR(F$12="", F$12="Prohibited")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F71:F86 G73:G82">
-    <cfRule type="expression" dxfId="50" priority="37">
+    <cfRule type="expression" dxfId="47" priority="37">
       <formula>OR(F$12="", F$12="Prohibited")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F92:F107 G94:G103">
-    <cfRule type="expression" dxfId="49" priority="12">
+    <cfRule type="expression" dxfId="46" priority="12">
       <formula>OR(F$12="", F$12="Prohibited")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G85:G89 F87:F89">
-    <cfRule type="expression" dxfId="48" priority="39" stopIfTrue="1">
+    <cfRule type="expression" dxfId="45" priority="39" stopIfTrue="1">
       <formula>OR(F$13="", F$13="Prohibited")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G106:G110 F108:F110">
-    <cfRule type="expression" dxfId="47" priority="14" stopIfTrue="1">
+    <cfRule type="expression" dxfId="44" priority="14" stopIfTrue="1">
       <formula>OR(F$13="", F$13="Prohibited")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G115:G120">
-    <cfRule type="expression" dxfId="46" priority="89" stopIfTrue="1">
+    <cfRule type="expression" dxfId="43" priority="89" stopIfTrue="1">
       <formula>OR(G$13="", G$13="Prohibited")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G121">
-    <cfRule type="expression" dxfId="45" priority="90">
+    <cfRule type="expression" dxfId="42" priority="90">
       <formula>OR(G$14="", G$14="Prohibited")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G127:G128">
-    <cfRule type="expression" dxfId="44" priority="51" stopIfTrue="1">
+    <cfRule type="expression" dxfId="41" priority="51" stopIfTrue="1">
       <formula>OR(G$13="", G$13="Prohibited")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G130:G132">
-    <cfRule type="expression" dxfId="43" priority="50" stopIfTrue="1">
+    <cfRule type="expression" dxfId="40" priority="50" stopIfTrue="1">
       <formula>OR(G$13="", G$13="Prohibited")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G135:G136">
-    <cfRule type="expression" dxfId="42" priority="86" stopIfTrue="1">
+    <cfRule type="expression" dxfId="39" priority="86" stopIfTrue="1">
       <formula>OR(G$13="", G$13="Prohibited")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H51:H66 I53:I62">
-    <cfRule type="expression" dxfId="41" priority="29">
+    <cfRule type="expression" dxfId="38" priority="29">
       <formula>OR(H$12="", H$12="Prohibited")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H71:H86 I73:I82">
-    <cfRule type="expression" dxfId="40" priority="26">
+    <cfRule type="expression" dxfId="37" priority="26">
       <formula>OR(H$12="", H$12="Prohibited")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H92:H107 I94:I103">
-    <cfRule type="expression" dxfId="39" priority="8">
+    <cfRule type="expression" dxfId="36" priority="8">
       <formula>OR(H$12="", H$12="Prohibited")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I85:I89 H87:H89">
-    <cfRule type="expression" dxfId="38" priority="28" stopIfTrue="1">
+    <cfRule type="expression" dxfId="35" priority="28" stopIfTrue="1">
       <formula>OR(H$13="", H$13="Prohibited")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I106:I110 H108:H110">
-    <cfRule type="expression" dxfId="37" priority="10" stopIfTrue="1">
+    <cfRule type="expression" dxfId="34" priority="10" stopIfTrue="1">
       <formula>OR(H$13="", H$13="Prohibited")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I115:I120">
-    <cfRule type="expression" dxfId="36" priority="81" stopIfTrue="1">
+    <cfRule type="expression" dxfId="33" priority="81" stopIfTrue="1">
       <formula>OR(I$13="", I$13="Prohibited")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I121">
-    <cfRule type="expression" dxfId="35" priority="82">
+    <cfRule type="expression" dxfId="32" priority="82">
       <formula>OR(I$14="", I$14="Prohibited")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I127:I128">
-    <cfRule type="expression" dxfId="34" priority="49" stopIfTrue="1">
+    <cfRule type="expression" dxfId="31" priority="49" stopIfTrue="1">
       <formula>OR(I$13="", I$13="Prohibited")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I130:I132">
-    <cfRule type="expression" dxfId="33" priority="48" stopIfTrue="1">
+    <cfRule type="expression" dxfId="30" priority="48" stopIfTrue="1">
       <formula>OR(I$13="", I$13="Prohibited")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I135:I136">
-    <cfRule type="expression" dxfId="32" priority="78" stopIfTrue="1">
+    <cfRule type="expression" dxfId="29" priority="78" stopIfTrue="1">
       <formula>OR(I$13="", I$13="Prohibited")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J92:J95 J102:J111">
-    <cfRule type="expression" dxfId="31" priority="18">
+    <cfRule type="expression" dxfId="28" priority="18">
       <formula>OR(J$14="", J$14="Prohibited")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J38:K43">
-    <cfRule type="expression" dxfId="30" priority="22" stopIfTrue="1">
+    <cfRule type="expression" dxfId="27" priority="22" stopIfTrue="1">
       <formula>OR(J$11="", J$11="Prohibited")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J55:K60">
-    <cfRule type="expression" dxfId="29" priority="21" stopIfTrue="1">
+    <cfRule type="expression" dxfId="26" priority="21" stopIfTrue="1">
       <formula>OR(J$11="", J$11="Prohibited")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J75:K80">
-    <cfRule type="expression" dxfId="28" priority="20" stopIfTrue="1">
+    <cfRule type="expression" dxfId="25" priority="20" stopIfTrue="1">
       <formula>OR(J$11="", J$11="Prohibited")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J96:K101">
-    <cfRule type="expression" dxfId="27" priority="16" stopIfTrue="1">
+    <cfRule type="expression" dxfId="24" priority="16" stopIfTrue="1">
       <formula>OR(J$11="", J$11="Prohibited")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K73:K74 K81:K82 K85:K89">
-    <cfRule type="expression" dxfId="26" priority="77" stopIfTrue="1">
+    <cfRule type="expression" dxfId="23" priority="77" stopIfTrue="1">
       <formula>OR(K$13="", K$13="Prohibited")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K94:K95 K102:K103 K106:K110">
-    <cfRule type="expression" dxfId="25" priority="17" stopIfTrue="1">
+    <cfRule type="expression" dxfId="22" priority="17" stopIfTrue="1">
       <formula>OR(K$13="", K$13="Prohibited")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K115:K120">
-    <cfRule type="expression" dxfId="24" priority="73" stopIfTrue="1">
+    <cfRule type="expression" dxfId="21" priority="73" stopIfTrue="1">
       <formula>OR(K$13="", K$13="Prohibited")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K121">
-    <cfRule type="expression" dxfId="23" priority="74">
+    <cfRule type="expression" dxfId="20" priority="74">
       <formula>OR(K$14="", K$14="Prohibited")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K127:K128">
-    <cfRule type="expression" dxfId="22" priority="47" stopIfTrue="1">
+    <cfRule type="expression" dxfId="19" priority="47" stopIfTrue="1">
       <formula>OR(K$13="", K$13="Prohibited")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K130:K132">
-    <cfRule type="expression" dxfId="21" priority="46" stopIfTrue="1">
+    <cfRule type="expression" dxfId="18" priority="46" stopIfTrue="1">
       <formula>OR(K$13="", K$13="Prohibited")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K135:K136">
-    <cfRule type="expression" dxfId="20" priority="70" stopIfTrue="1">
+    <cfRule type="expression" dxfId="17" priority="70" stopIfTrue="1">
       <formula>OR(K$13="", K$13="Prohibited")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K111:O111">
-    <cfRule type="expression" dxfId="19" priority="6">
+    <cfRule type="expression" dxfId="16" priority="6">
       <formula>OR(K$14="", K$14="Prohibited")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L71:L73 N71:N73 J71:J74 B71:B89 D71:D90 P71:T90 J81:J90 B90:C90 E90:I90 K90:O90">
-    <cfRule type="expression" dxfId="18" priority="276">
+  <conditionalFormatting sqref="L71:L73 N71:N73 J71:J74 B71:B89 D71:D90 J81:J90 B90:C90 E90:I90 K90:O90">
+    <cfRule type="expression" dxfId="15" priority="276">
       <formula>OR(B$14="", B$14="Prohibited")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L92:L95 N92:N95 B92:B111 D92:D111 P92:T111">
-    <cfRule type="expression" dxfId="17" priority="275" stopIfTrue="1">
+  <conditionalFormatting sqref="L92:L95 N92:N95 B92:B111 D92:D111">
+    <cfRule type="expression" dxfId="14" priority="275" stopIfTrue="1">
       <formula>OR(B$15="", B$15="Prohibited")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M73:M82 L74:L89 M85:M89">
-    <cfRule type="expression" dxfId="16" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="13" priority="7" stopIfTrue="1">
       <formula>OR(L$13="", L$13="Prohibited")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M94:M103 L96:L110 M106:M110">
-    <cfRule type="expression" dxfId="15" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="12" priority="5" stopIfTrue="1">
       <formula>OR(L$13="", L$13="Prohibited")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M115:M120">
-    <cfRule type="expression" dxfId="14" priority="62" stopIfTrue="1">
+    <cfRule type="expression" dxfId="11" priority="62" stopIfTrue="1">
       <formula>OR(M$13="", M$13="Prohibited")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M121">
-    <cfRule type="expression" dxfId="13" priority="63">
+    <cfRule type="expression" dxfId="10" priority="63">
       <formula>OR(M$14="", M$14="Prohibited")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M127:M128">
-    <cfRule type="expression" dxfId="12" priority="45" stopIfTrue="1">
+    <cfRule type="expression" dxfId="9" priority="45" stopIfTrue="1">
       <formula>OR(M$13="", M$13="Prohibited")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M130:M132">
-    <cfRule type="expression" dxfId="11" priority="44" stopIfTrue="1">
+    <cfRule type="expression" dxfId="8" priority="44" stopIfTrue="1">
       <formula>OR(M$13="", M$13="Prohibited")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M135:M136">
-    <cfRule type="expression" dxfId="10" priority="55" stopIfTrue="1">
+    <cfRule type="expression" dxfId="7" priority="55" stopIfTrue="1">
       <formula>OR(M$13="", M$13="Prohibited")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O73:O82 N74:N89 O85:O89">
-    <cfRule type="expression" dxfId="9" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="6" priority="3" stopIfTrue="1">
       <formula>OR(N$13="", N$13="Prohibited")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O94:O103 N96:N110 O106:O110">
-    <cfRule type="expression" dxfId="8" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="5" priority="1" stopIfTrue="1">
       <formula>OR(N$13="", N$13="Prohibited")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O115:O120">
-    <cfRule type="expression" dxfId="7" priority="60" stopIfTrue="1">
+    <cfRule type="expression" dxfId="4" priority="60" stopIfTrue="1">
       <formula>OR(O$13="", O$13="Prohibited")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O121">
-    <cfRule type="expression" dxfId="6" priority="61">
+    <cfRule type="expression" dxfId="3" priority="61">
       <formula>OR(O$14="", O$14="Prohibited")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O127:O128">
-    <cfRule type="expression" dxfId="5" priority="43" stopIfTrue="1">
+    <cfRule type="expression" dxfId="2" priority="43" stopIfTrue="1">
       <formula>OR(O$13="", O$13="Prohibited")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O130:O132">
-    <cfRule type="expression" dxfId="4" priority="42" stopIfTrue="1">
+    <cfRule type="expression" dxfId="1" priority="42" stopIfTrue="1">
       <formula>OR(O$13="", O$13="Prohibited")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O135:O136">
-    <cfRule type="expression" dxfId="3" priority="54" stopIfTrue="1">
+    <cfRule type="expression" dxfId="0" priority="54" stopIfTrue="1">
       <formula>OR(O$13="", O$13="Prohibited")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B114:B121 D114:D121 F114:F121 H114:H121 J114:J121 L114:L121 N114:N121 P114:T121">
-    <cfRule type="expression" dxfId="2" priority="274" stopIfTrue="1">
-      <formula>OR(B$17="", B$17="Prohibited")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B123:B132 D123:D132 F123:F132 H123:H132 J123:J132 L123:L132 N123:N132 P123:T132">
-    <cfRule type="expression" dxfId="1" priority="273">
-      <formula>OR(B$16="", B$16="Prohibited")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B134:B137 D134:D137 F134:F137 H134:H137 J134:J137 L134:L137 N134:N137 P134:T137">
-    <cfRule type="expression" dxfId="0" priority="272" stopIfTrue="1">
-      <formula>OR(B$18="Prohibited", B$18="")</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6501,13 +6439,13 @@
           <x14:formula1>
             <xm:f>Sheet2!$A$1:$A$2</xm:f>
           </x14:formula1>
-          <xm:sqref>B34:B35 C104:C105 C71:C72 C83:C84 C92:C93 H51:H52 M71:M72 M92:M93 I104:I105 P34:T35 D34:D35 F34:F35 J34:J35 L34:L35 H92:H93 E92:F93 E104:E105 E71:F72 E83:E84 B63:E64 G83:G84 B51:F52 K71:K72 K83:O84 K92:K93 K104:O105 O71:O72 G104:G105 G63:G64 N34:N35 H34:H35 H71:H72 I83:I84 O92:O93 B134:T134 B139:T139 B9:U10 B141:T142 J51:T52 I63:T64 B5:U7</xm:sqref>
+          <xm:sqref>B34:B35 C104:C105 C71:C72 C83:C84 C92:C93 H51:H52 M71:M72 M92:M93 I104:I105 D34:D35 F34:F35 J34:J35 L34:L35 H92:H93 E92:F93 E104:E105 E71:F72 E83:E84 B63:E64 G83:G84 B51:F52 K71:K72 K83:O84 K92:K93 K104:O105 O71:O72 G104:G105 G63:G64 N34:N35 H34:H35 H71:H72 I83:I84 O92:O93 B134:O134 B139:O139 B141:O142 J51:O52 I63:O64 B5:P7 B9:P10</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{271A050A-B09A-2046-9CFC-53A5B24425CC}">
           <x14:formula1>
             <xm:f>Sheet2!$B$1:$B$5</xm:f>
           </x14:formula1>
-          <xm:sqref>B20 B16:B18 C16:C20 D16:D18 D20 F16:F18 F20 E16:E20 H16:H18 H20 G16:G20 J16:J18 J20 I16:I20 L16:L18 L20 M16:M20 N16:N18 N20 K16:K20 O16:U20</xm:sqref>
+          <xm:sqref>B20 B16:B18 C16:C20 D16:D18 D20 F16:F18 F20 E16:E20 H16:H18 H20 G16:G20 J16:J18 J20 I16:I20 L16:L18 L20 M16:M20 N16:N18 N20 K16:K20 O16:P20</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{19EF20F5-834F-4D48-B6E7-653C3CEE4371}">
           <x14:formula1>
@@ -6579,25 +6517,25 @@
           <x14:formula1>
             <xm:f>Sheet2!AA1:AA2</xm:f>
           </x14:formula1>
-          <xm:sqref>V5:W6</xm:sqref>
+          <xm:sqref>Q5:R6</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{4451BF94-E622-3245-ADEB-7B90297251C3}">
           <x14:formula1>
             <xm:f>Sheet2!$B$1:$B$4</xm:f>
           </x14:formula1>
-          <xm:sqref>B12:U15 B11:Y11</xm:sqref>
+          <xm:sqref>B11:T11 B12:P15</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{FEF44111-19BE-8543-99E7-8B474E6AA7E3}">
           <x14:formula1>
             <xm:f>Sheet2!B3:B4</xm:f>
           </x14:formula1>
-          <xm:sqref>C8 E8 G8 I8 M8 O8 K8</xm:sqref>
+          <xm:sqref>C8 K8 O8 M8 I8 G8 E8</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{44745D1C-7B97-1941-8A45-35D0341299F6}">
           <x14:formula1>
-            <xm:f>Sheet2!U3:U4</xm:f>
+            <xm:f>Sheet2!Z3:Z4</xm:f>
           </x14:formula1>
-          <xm:sqref>P8:U8</xm:sqref>
+          <xm:sqref>P8</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -6609,7 +6547,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05389331-E65F-9747-B96F-F1FC2DF92AD8}">
   <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
@@ -6729,7 +6667,7 @@
       <c r="A12" t="s">
         <v>102</v>
       </c>
-      <c r="B12" s="6">
+      <c r="B12" s="5">
         <v>41702</v>
       </c>
     </row>
@@ -6737,7 +6675,7 @@
       <c r="A13" t="s">
         <v>103</v>
       </c>
-      <c r="B13" s="6">
+      <c r="B13" s="5">
         <v>41338</v>
       </c>
     </row>

</xml_diff>